<commit_message>
correct syntactical errors in NGC code and add Makefiles
</commit_message>
<xml_diff>
--- a/apps/eop1/MA_v0.7_dist/MA_v0.7_doc/MA_v0.7_DataModel.xlsx
+++ b/apps/eop1/MA_v0.7_dist/MA_v0.7_doc/MA_v0.7_DataModel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MA_v0.7_dist\MA_v0.7_doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\gaps\MA_v0.7_dist\MA_v0.7_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3A7340-8215-4ED4-BD22-BB419DBEB423}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conceptual" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="106">
   <si>
     <t>PNT</t>
   </si>
@@ -527,12 +528,51 @@
   <si>
     <t>100ms during startup only</t>
   </si>
+  <si>
+    <t>groundMovers</t>
+  </si>
+  <si>
+    <t>No publisher</t>
+  </si>
+  <si>
+    <t>Incorrect Receiver (ISRM, instead of MPU)</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>1 Hz (comment says 100Hz)</t>
+  </si>
+  <si>
+    <t>No Listener (messages stopped after the first 50 received in 400 seconds)</t>
+  </si>
+  <si>
+    <t>No wait between sending messages; repeated call to amq.listen</t>
+  </si>
+  <si>
+    <t>Not listed; Queue, all others are Topic</t>
+  </si>
+  <si>
+    <r>
+      <t>EVERY UNIT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ except MPU</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,16 +631,47 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -623,11 +694,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -663,9 +745,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -683,6 +762,37 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -719,7 +829,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="26" name="Elbow Connector 25"/>
+        <xdr:cNvPr id="26" name="Elbow Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -768,7 +884,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="29" name="Elbow Connector 28"/>
+        <xdr:cNvPr id="29" name="Elbow Connector 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -817,7 +939,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="Elbow Connector 29"/>
+        <xdr:cNvPr id="30" name="Elbow Connector 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -866,7 +994,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="31" name="Elbow Connector 30"/>
+        <xdr:cNvPr id="31" name="Elbow Connector 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -915,7 +1049,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="32" name="Elbow Connector 31"/>
+        <xdr:cNvPr id="32" name="Elbow Connector 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000020000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -964,7 +1104,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="43" name="Elbow Connector 42"/>
+        <xdr:cNvPr id="43" name="Elbow Connector 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1013,7 +1159,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="47" name="Elbow Connector 46"/>
+        <xdr:cNvPr id="47" name="Elbow Connector 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1062,7 +1214,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="53" name="Elbow Connector 52"/>
+        <xdr:cNvPr id="53" name="Elbow Connector 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000035000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1111,7 +1269,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="59" name="Elbow Connector 58"/>
+        <xdr:cNvPr id="59" name="Elbow Connector 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00003B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1157,7 +1321,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="67" name="Elbow Connector 66"/>
+        <xdr:cNvPr id="67" name="Elbow Connector 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000043000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1456,33 +1626,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="3" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" customWidth="1"/>
-    <col min="9" max="9" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
-    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.44140625" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
@@ -1500,10 +1670,10 @@
       </c>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:16" ht="153" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="153" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1525,15 +1695,15 @@
       <c r="L3" s="3"/>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:16" ht="144.6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="150.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1555,15 +1725,15 @@
       <c r="L6" s="3"/>
       <c r="P6" s="3"/>
     </row>
-    <row r="7" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:16" ht="101.4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="105.75" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1585,15 +1755,15 @@
       <c r="L9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1615,15 +1785,15 @@
       <c r="L12" s="3"/>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:16" ht="58.2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1645,13 +1815,13 @@
       <c r="L15" s="3"/>
       <c r="P15" s="3"/>
     </row>
-    <row r="16" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:16" ht="29.4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" ht="45.75" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1672,13 +1842,13 @@
       </c>
       <c r="P18" s="3"/>
     </row>
-    <row r="19" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -1690,30 +1860,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="5"/>
-    <col min="4" max="4" width="11.88671875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="5"/>
-    <col min="7" max="7" width="16.88671875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5546875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="19.88671875" style="5" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="5"/>
+    <col min="1" max="1" width="15.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="5"/>
+    <col min="4" max="4" width="11.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="5"/>
+    <col min="7" max="7" width="16.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" style="5" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>51</v>
       </c>
@@ -1748,7 +1918,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>69</v>
       </c>
@@ -1777,7 +1947,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1806,7 +1976,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1835,7 +2005,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
@@ -1864,7 +2034,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
@@ -1893,7 +2063,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>66</v>
       </c>
@@ -1919,7 +2089,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>66</v>
       </c>
@@ -1945,7 +2115,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>2</v>
       </c>
@@ -1971,7 +2141,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>2</v>
       </c>
@@ -1997,7 +2167,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>3</v>
       </c>
@@ -2023,7 +2193,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -2049,7 +2219,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
@@ -2075,57 +2245,57 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I15"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I17"/>
     </row>
-    <row r="18" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I18"/>
     </row>
-    <row r="19" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I20"/>
     </row>
-    <row r="21" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I21"/>
     </row>
-    <row r="22" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I23"/>
     </row>
-    <row r="24" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I24"/>
     </row>
-    <row r="25" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I26"/>
     </row>
-    <row r="27" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I27"/>
     </row>
-    <row r="28" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I28" s="3"/>
     </row>
-    <row r="32" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="9:20" x14ac:dyDescent="0.25">
       <c r="T32" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="18:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="18:22" x14ac:dyDescent="0.25">
       <c r="R36" s="5" t="s">
         <v>1</v>
       </c>
@@ -2133,17 +2303,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="18:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="18:22" x14ac:dyDescent="0.25">
       <c r="U39" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="18:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="18:22" x14ac:dyDescent="0.25">
       <c r="T40" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="18:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="18:22" x14ac:dyDescent="0.25">
       <c r="S41" s="5" t="s">
         <v>2</v>
       </c>
@@ -2156,23 +2326,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="32.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" customWidth="1"/>
+    <col min="6" max="6" width="40.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>78</v>
       </c>
@@ -2188,59 +2359,68 @@
       <c r="E1" s="8" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="140.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="F1" s="26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="64.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="F2" s="25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>84</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="F3" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="17" t="s">
+      <c r="C4" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="22" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -2250,31 +2430,34 @@
       <c r="C5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>92</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>89</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>90</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="F6" s="25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>94</v>
       </c>
@@ -2284,12 +2467,35 @@
       <c r="C7" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="30" t="s">
         <v>96</v>
       </c>
+      <c r="F7" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>